<commit_message>
Add measurements from nPM1300
</commit_message>
<xml_diff>
--- a/docs/nPM1300 cost breakdown.xlsx
+++ b/docs/nPM1300 cost breakdown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git\ZSWatch-HW\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{345DD511-F4DB-4AA0-B313-C62F705D33B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7784089-FAF1-4034-88C0-1A5B0C150319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27060" yWindow="3405" windowWidth="22140" windowHeight="15345" xr2:uid="{D663AEF1-A208-4655-BFB8-7F952685C007}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{D663AEF1-A208-4655-BFB8-7F952685C007}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Power Supply &lt;= rev 3</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Delta</t>
   </si>
 </sst>
 </file>
@@ -114,7 +117,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,6 +139,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -154,18 +164,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -478,43 +491,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B676CE99-A328-4A2B-BE65-84AC1B49A40D}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="2"/>
+    <col min="2" max="2" width="11.42578125" style="1"/>
     <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>4.46</v>
       </c>
       <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>3.91</v>
       </c>
     </row>
@@ -522,13 +535,13 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>0.4</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>0.158</v>
       </c>
     </row>
@@ -536,13 +549,13 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>0.37</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>0.223</v>
       </c>
     </row>
@@ -550,13 +563,13 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>1.36</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>0.223</v>
       </c>
     </row>
@@ -564,13 +577,13 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>1.36</v>
       </c>
       <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
@@ -578,13 +591,13 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>0.13</v>
       </c>
       <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
@@ -592,13 +605,13 @@
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>0.223</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>0.27900000000000003</v>
       </c>
     </row>
@@ -606,13 +619,13 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>0.27900000000000003</v>
       </c>
     </row>
@@ -620,13 +633,13 @@
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>0.27900000000000003</v>
       </c>
     </row>
@@ -634,13 +647,13 @@
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>0.48399999999999999</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>0.27900000000000003</v>
       </c>
     </row>
@@ -648,13 +661,13 @@
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>0.36299999999999999</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <v>0.27900000000000003</v>
       </c>
     </row>
@@ -662,13 +675,13 @@
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>0.186</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>0.223</v>
       </c>
     </row>
@@ -676,13 +689,13 @@
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>0.34439999999999998</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <v>0.223</v>
       </c>
     </row>
@@ -690,48 +703,66 @@
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>0.20499999999999999</v>
       </c>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>0.19</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.34439999999999998</v>
+      </c>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>22</v>
       </c>
-      <c r="E16">
+      <c r="B20" s="1">
+        <f>SUM(B2:B18)</f>
+        <v>10.810800000000002</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="1">
         <f>SUM(E2:E14)</f>
         <v>6.5409999999999995</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="2">
-        <v>0.34439999999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="2">
-        <v>0.20499999999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="2">
-        <f>SUM(B2:B18)</f>
-        <v>10.810800000000002</v>
+      <c r="G20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="1">
+        <f>B20-E20</f>
+        <v>4.2698000000000027</v>
+      </c>
+      <c r="I20" s="4">
+        <f>E20/B20</f>
+        <v>0.60504310504310488</v>
       </c>
     </row>
   </sheetData>

</xml_diff>